<commit_message>
adding additional rows to provisional database
</commit_message>
<xml_diff>
--- a/biking_provisional_db.xlsx
+++ b/biking_provisional_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RyanCook/Desktop/Data_Bootcamp_Capstone_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6950A32-F099-6946-BEB5-FF494B4E04EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B005116-AEA9-6947-B330-DD2C09CBA47C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6220" yWindow="520" windowWidth="21740" windowHeight="15420" activeTab="2" xr2:uid="{488E7AC1-42C5-7342-9085-A2E225B3B33B}"/>
+    <workbookView xWindow="6220" yWindow="520" windowWidth="21740" windowHeight="15420" xr2:uid="{488E7AC1-42C5-7342-9085-A2E225B3B33B}"/>
   </bookViews>
   <sheets>
     <sheet name="joined_db" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="20">
   <si>
     <t>date</t>
   </si>
@@ -89,13 +89,13 @@
     <t>Shared Use Path</t>
   </si>
   <si>
-    <t>etc.</t>
-  </si>
-  <si>
     <t>total_bikers</t>
   </si>
   <si>
     <t>total_pedestrians</t>
+  </si>
+  <si>
+    <t>…</t>
   </si>
 </sst>
 </file>
@@ -448,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{188829EE-9332-1441-9FB8-CA75659B8B52}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,10 +497,10 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
         <v>18</v>
-      </c>
-      <c r="L1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -580,8 +580,768 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>17</v>
+      <c r="A4" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>285.45</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4">
+        <v>2031</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4">
+        <v>129</v>
+      </c>
+      <c r="L4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E5">
+        <v>1.3</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>99</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5">
+        <v>1371</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>285.45</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6">
+        <v>2031</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6">
+        <v>129</v>
+      </c>
+      <c r="L6">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E7">
+        <v>1.3</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>99</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7">
+        <v>1371</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>285.45</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8">
+        <v>2031</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8">
+        <v>129</v>
+      </c>
+      <c r="L8">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E9">
+        <v>1.3</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>99</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9">
+        <v>1371</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>285.45</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10">
+        <v>2031</v>
+      </c>
+      <c r="J10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10">
+        <v>129</v>
+      </c>
+      <c r="L10">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E11">
+        <v>1.3</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>99</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11">
+        <v>1371</v>
+      </c>
+      <c r="J11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>285.45</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12">
+        <v>2031</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12">
+        <v>129</v>
+      </c>
+      <c r="L12">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E13">
+        <v>1.3</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>99</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13">
+        <v>1371</v>
+      </c>
+      <c r="J13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>285.45</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14">
+        <v>2031</v>
+      </c>
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14">
+        <v>129</v>
+      </c>
+      <c r="L14">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E15">
+        <v>1.3</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>99</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15">
+        <v>1371</v>
+      </c>
+      <c r="J15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>285.45</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16">
+        <v>2031</v>
+      </c>
+      <c r="J16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16">
+        <v>129</v>
+      </c>
+      <c r="L16">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E17">
+        <v>1.3</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>99</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17">
+        <v>1371</v>
+      </c>
+      <c r="J17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>285.45</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18">
+        <v>2031</v>
+      </c>
+      <c r="J18" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18">
+        <v>129</v>
+      </c>
+      <c r="L18">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E19">
+        <v>1.3</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>99</v>
+      </c>
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19">
+        <v>1371</v>
+      </c>
+      <c r="J19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>285.45</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20">
+        <v>2031</v>
+      </c>
+      <c r="J20" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20">
+        <v>129</v>
+      </c>
+      <c r="L20">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E21">
+        <v>1.3</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>99</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21">
+        <v>1371</v>
+      </c>
+      <c r="J21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>285.45</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22">
+        <v>2031</v>
+      </c>
+      <c r="J22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22">
+        <v>129</v>
+      </c>
+      <c r="L22">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E23">
+        <v>1.3</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>99</v>
+      </c>
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23">
+        <v>1371</v>
+      </c>
+      <c r="J23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -591,10 +1351,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11BE4AEF-9218-8048-B415-2A09F9C78B19}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -693,6 +1453,707 @@
         <v>1371</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>285.45</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E5">
+        <v>1.3</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>99</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>285.45</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E7">
+        <v>1.3</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>99</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>285.45</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E9">
+        <v>1.3</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>99</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>285.45</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E11">
+        <v>1.3</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>99</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>285.45</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E13">
+        <v>1.3</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>99</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>285.45</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E15">
+        <v>1.3</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>99</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>285.45</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E17">
+        <v>1.3</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>99</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>285.45</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E19">
+        <v>1.3</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>99</v>
+      </c>
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>285.45</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E21">
+        <v>1.3</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>99</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>285.45</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E23">
+        <v>1.3</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>99</v>
+      </c>
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24">
+        <v>285.45</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E25">
+        <v>1.3</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>99</v>
+      </c>
+      <c r="H25" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>285.45</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="E27">
+        <v>1.3</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>99</v>
+      </c>
+      <c r="H27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -700,10 +2161,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A76F6F-A1EA-0D49-8983-15ABB936F085}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -721,10 +2182,10 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -753,6 +2214,319 @@
       </c>
       <c r="D3">
         <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>129</v>
+      </c>
+      <c r="D4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>129</v>
+      </c>
+      <c r="D6">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>129</v>
+      </c>
+      <c r="D8">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>129</v>
+      </c>
+      <c r="D10">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>129</v>
+      </c>
+      <c r="D12">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>129</v>
+      </c>
+      <c r="D14">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>129</v>
+      </c>
+      <c r="D16">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>129</v>
+      </c>
+      <c r="D18">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <v>129</v>
+      </c>
+      <c r="D20">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>129</v>
+      </c>
+      <c r="D22">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>129</v>
+      </c>
+      <c r="D24">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>